<commit_message>
add hidden variables in O100011
</commit_message>
<xml_diff>
--- a/Mould_Database/Mould_Cal.xlsx
+++ b/Mould_Database/Mould_Cal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Documents\GitHub\mould\Mould_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925FF39A-2247-4EED-BA94-C73A588209D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1796B3D-7D59-48D8-AFB7-E664858DBBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="638" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
+    <workbookView xWindow="0" yWindow="525" windowWidth="17235" windowHeight="15075" tabRatio="638" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
   </bookViews>
   <sheets>
     <sheet name="position" sheetId="17" r:id="rId1"/>
@@ -11753,113 +11753,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>-C48</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>sqrt{R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>-(f</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>-C48)</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>}</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>トップ外削外径AC</t>
     <rPh sb="3" eb="5">
       <t>ガイサク</t>
@@ -12275,6 +12168,113 @@
     <rPh sb="17" eb="19">
       <t>チュウシン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>-C49</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>sqrt{R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>-(f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>-C49)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>}</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -13100,6 +13100,62 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -13276,62 +13332,6 @@
       <font>
         <strike val="0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -13749,7 +13749,9 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:R170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
@@ -14695,7 +14697,7 @@
         <v>357</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C23" s="59">
         <v>102</v>
@@ -14738,7 +14740,7 @@
         <v>358</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C24" s="59">
         <v>85</v>
@@ -14827,7 +14829,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B26" s="58" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C26" s="63">
         <v>40</v>
@@ -14863,7 +14865,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B27" s="58" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C27" s="63">
         <v>32</v>
@@ -14904,10 +14906,10 @@
         <v>28</v>
       </c>
       <c r="L28" s="89" t="s">
-        <v>436</v>
+        <v>462</v>
       </c>
       <c r="M28" s="98" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="N28" s="46">
         <f>$C$5-$C$49</f>
@@ -14937,10 +14939,10 @@
         <v>29</v>
       </c>
       <c r="L29" s="89" t="s">
-        <v>437</v>
+        <v>463</v>
       </c>
       <c r="M29" s="98" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="N29" s="46">
         <f>SQRT($C$3^2-$N$28^2)</f>
@@ -15284,7 +15286,7 @@
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B40" s="58" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C40" s="77">
         <v>180.95</v>
@@ -15481,7 +15483,7 @@
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B46" s="48" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F46" s="68"/>
       <c r="G46" s="66"/>
@@ -15665,7 +15667,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B52" s="48" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>275</v>
@@ -15700,7 +15702,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="76" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="K53" s="47">
         <f t="shared" si="0"/>
@@ -16265,7 +16267,7 @@
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B69" s="45" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C69" s="49">
         <v>-561.11400000000003</v>
@@ -16304,7 +16306,7 @@
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B70" s="45" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C70" s="49">
         <v>-648.33199999999999</v>
@@ -16579,7 +16581,7 @@
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.4">
       <c r="F79" s="76" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K79" s="47">
         <f t="shared" si="2"/>
@@ -16985,7 +16987,7 @@
     </row>
     <row r="94" spans="6:14" x14ac:dyDescent="0.4">
       <c r="F94" s="54" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G94" s="57" t="s">
         <v>177</v>
@@ -17011,7 +17013,7 @@
     </row>
     <row r="95" spans="6:14" x14ac:dyDescent="0.4">
       <c r="F95" s="54" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G95" s="57" t="s">
         <v>177</v>
@@ -17053,10 +17055,10 @@
     </row>
     <row r="97" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E97" s="47" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F97" s="53" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G97" s="57" t="s">
         <v>180</v>
@@ -17086,10 +17088,10 @@
     </row>
     <row r="98" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E98" s="47" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F98" s="53" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G98" s="57" t="s">
         <v>177</v>
@@ -17119,10 +17121,10 @@
     </row>
     <row r="99" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E99" s="47" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F99" s="53" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G99" s="57" t="s">
         <v>180</v>
@@ -17152,10 +17154,10 @@
     </row>
     <row r="100" spans="5:14" x14ac:dyDescent="0.4">
       <c r="E100" s="47" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F100" s="53" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G100" s="57" t="s">
         <v>177</v>
@@ -17173,10 +17175,10 @@
         <v>100</v>
       </c>
       <c r="L100" s="89" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="M100" s="98" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="N100" s="46">
         <f ca="1">SIN(RADIANS($H$73))</f>
@@ -17185,7 +17187,7 @@
     </row>
     <row r="101" spans="5:14" x14ac:dyDescent="0.4">
       <c r="F101" s="53" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G101" s="57" t="s">
         <v>180</v>
@@ -17199,10 +17201,10 @@
         <v>101</v>
       </c>
       <c r="L101" s="89" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="M101" s="98" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="N101" s="46">
         <f ca="1">COS(RADIANS($H$73))</f>
@@ -17211,7 +17213,7 @@
     </row>
     <row r="102" spans="5:14" x14ac:dyDescent="0.4">
       <c r="F102" s="53" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G102" s="57" t="s">
         <v>177</v>
@@ -18063,190 +18065,190 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="46" priority="123">
+    <cfRule type="expression" dxfId="54" priority="123">
       <formula>$C$3&gt;2*N151</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="45" priority="43">
+    <cfRule type="expression" dxfId="53" priority="43">
       <formula>C4&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="44" priority="19">
+    <cfRule type="expression" dxfId="52" priority="19">
       <formula>$C$6&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="43" priority="47">
+    <cfRule type="expression" dxfId="51" priority="47">
       <formula>$C$9&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C11">
-    <cfRule type="expression" dxfId="42" priority="20">
+    <cfRule type="expression" dxfId="50" priority="20">
       <formula>$C$10&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="41" priority="98">
+    <cfRule type="expression" dxfId="49" priority="98">
       <formula>OR(C15&lt;=0, C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="40" priority="42">
+    <cfRule type="expression" dxfId="48" priority="42">
       <formula>C35&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="39" priority="57">
+    <cfRule type="expression" dxfId="47" priority="57">
       <formula>OR($C$36&lt;0, $C$36&gt;=$C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="38" priority="16">
+    <cfRule type="expression" dxfId="46" priority="16">
       <formula>OR($C$37&lt;0, $C$37&gt;=$C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="37" priority="120">
+    <cfRule type="expression" dxfId="45" priority="120">
       <formula>OR(C38&lt;0, C38&gt;=C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="36" priority="127">
+    <cfRule type="expression" dxfId="44" priority="127">
       <formula>OR(C39&lt;0, C39&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="35" priority="128">
+    <cfRule type="expression" dxfId="43" priority="128">
       <formula>OR(C42&lt;0, C42&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="34" priority="51">
+    <cfRule type="expression" dxfId="42" priority="51">
       <formula>AND(C59&lt;&gt;330, C59&lt;&gt;270, C59&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="33" priority="50">
+    <cfRule type="expression" dxfId="41" priority="50">
       <formula>C60&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="32" priority="27">
+    <cfRule type="expression" dxfId="40" priority="27">
       <formula>OR(C63&gt;0, ABS(ABS(C63)-740)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="31" priority="40">
+    <cfRule type="expression" dxfId="39" priority="40">
       <formula>OR(C64&gt;0, ABS(ABS(C64)-550)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="30" priority="33">
+    <cfRule type="expression" dxfId="38" priority="33">
       <formula>OR(C65&gt;0, ABS(ABS(C65)-1150)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="29" priority="39">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>OR(ABS(C66)&gt;=0.2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="28" priority="23">
+    <cfRule type="expression" dxfId="36" priority="23">
       <formula>OR($H$48&lt;=1, INT($H$48)&lt;&gt;$H$48)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="27" priority="15">
+    <cfRule type="expression" dxfId="35" priority="15">
       <formula>ISERROR(INDIRECT($H$52&amp;"!$G$45"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="26" priority="236">
+    <cfRule type="expression" dxfId="34" priority="236">
       <formula>OR(C25-QUOTIENT(C25,1)&lt;&gt;0, C25&lt;0, C25&gt;$C$67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="25" priority="11">
+    <cfRule type="expression" dxfId="33" priority="11">
       <formula>$H$50&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78 H51:H52 H54:H72">
-    <cfRule type="expression" dxfId="24" priority="10">
+    <cfRule type="expression" dxfId="32" priority="10">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="23" priority="254">
+    <cfRule type="expression" dxfId="31" priority="254">
       <formula>OR($C$23&lt;=0, MOD($C$23,$C$22)&lt;&gt;0, $C$23&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="22" priority="262">
+    <cfRule type="expression" dxfId="30" priority="262">
       <formula>OR($C$26&lt;=0, $C$26&gt;=MIN($C$23, $C$24))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:N133">
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:N141">
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="19" priority="274">
+    <cfRule type="expression" dxfId="27" priority="274">
       <formula>OR(C16&lt;=0, C16+C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="26" priority="3">
       <formula>G1="X"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>G1="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="24" priority="5">
       <formula>G1="Z"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="23" priority="6">
       <formula>G1="B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80:H95">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="13" priority="276">
+    <cfRule type="expression" dxfId="21" priority="276">
       <formula>OR($C$13&gt;=$C$9, $C$13&gt;=$C$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="12" priority="277">
+    <cfRule type="expression" dxfId="20" priority="277">
       <formula>OR($C$14&gt;=$C$10, $C$14&gt;=$C$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="11" priority="278">
+    <cfRule type="expression" dxfId="19" priority="278">
       <formula>OR($C$17&lt;=0, $C$17&gt;=($C$9-#REF!)/2, $C$17&gt;=($C$36-#REF!)/2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="10" priority="279">
+    <cfRule type="expression" dxfId="18" priority="279">
       <formula>$H$77&lt;=$C$27/2+$C$28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>OR($C$27&lt;=0, $C$27&gt;$C$26)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58:C67 H78 N128:N141 C47:C50 C53:C56 H54:H72 H80:H95 C3:C32 G1:G1048576" xr:uid="{5A8FA8E9-E7FC-48D2-B40E-E90D3C7D1F03}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20418,12 +20420,12 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:D42">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:N42">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21286,42 +21288,42 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="54" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>G9^2&lt;4*G10^2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="53" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>$C$4&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="52" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>C5&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="51" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>OR(C5&gt;C6, C6&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="50" priority="9">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>AND(C7&lt;&gt;330, C7&lt;&gt;270, C7&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="49" priority="8">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>C8&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="48" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>C9&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K4">
-    <cfRule type="expression" dxfId="47" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>OR(($K$8&gt;($C$5+$C$6-2*$C$7)),$K$3&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>